<commit_message>
cleaned up code for unique together constaint and string representation of Product_Name, Product_Type, and Product. Also added and debugged the excel sheets
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/pharma_pos.product.xlsx
+++ b/addons/pharma-pos/demo_excel/pharma_pos.product.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t xml:space="preserve">Med</t>
   </si>
@@ -49,10 +49,13 @@
     <t xml:space="preserve">Colchisin (Colchi)</t>
   </si>
   <si>
-    <t xml:space="preserve">20 cc Tablet</t>
+    <t xml:space="preserve">500 mg Tablet</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 cc Injection</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -92,6 +95,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -147,6 +156,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -166,13 +183,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="30.71"/>
   </cols>
@@ -212,8 +229,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -227,6 +244,23 @@
       </c>
       <c r="E3" s="2" t="n">
         <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more records to the excel demo
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/pharma_pos.product.xlsx
+++ b/addons/pharma-pos/demo_excel/pharma_pos.product.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">Med</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">Size</t>
@@ -43,19 +43,16 @@
     <t xml:space="preserve">10 mg Tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Colchisin (Colchi)</t>
   </si>
   <si>
     <t xml:space="preserve">500 mg Tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
     <t xml:space="preserve">20 cc Injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Losartan (Lora)</t>
   </si>
 </sst>
 </file>
@@ -65,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,12 +92,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,7 +136,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,14 +147,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -183,18 +166,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="30.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -218,49 +201,81 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed previous demo data and added one record for each model
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/pharma_pos.product.xlsx
+++ b/addons/pharma-pos/demo_excel/pharma_pos.product.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -37,22 +37,10 @@
     <t xml:space="preserve">Is Sold</t>
   </si>
   <si>
-    <t xml:space="preserve">Atenolol (Ate)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 mg Tablet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colchisin (Colchi)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500 mg Tablet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 cc Injection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Losartan (Lora)</t>
+    <t xml:space="preserve">Aciclovir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 mg Tablet</t>
   </si>
 </sst>
 </file>
@@ -169,10 +157,10 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="30.71"/>
   </cols>
@@ -194,7 +182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -211,74 +199,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>